<commit_message>
changed plate reader import template variable to target
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFE4567-0DDE-3D4A-B105-42016946D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC05C5A-F91C-DE43-B32D-BCBD72AB4238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>replicate</t>
   </si>
   <si>
-    <t>cell_line</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>conc_uM</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>$B$2</f>
@@ -648,7 +648,7 @@
         <v>NA</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:L8" si="2">$C$3</f>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <f>B$1</f>
@@ -1126,7 +1126,7 @@
         <v>NA</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="e">
         <f>C13/3</f>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <f>B$1</f>
@@ -1609,7 +1609,7 @@
         <v>NA</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ref="D23:L25" si="13">$C$23</f>
@@ -1770,7 +1770,7 @@
         <v>NA</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" ref="D26:L28" si="14">$C$26</f>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <f>B$1</f>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41">
         <f>B$1</f>

</xml_diff>

<commit_message>
Updated import template with more options for complicated experiments, plus automatic coloring for catching errors
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC05C5A-F91C-DE43-B32D-BCBD72AB4238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D87DD0-C847-0B47-952C-D96C5AB2047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1236,11 +1236,11 @@
         <v>initial conc (uM)</v>
       </c>
       <c r="D15" t="e">
-        <f t="shared" si="9"/>
+        <f>D$13</f>
         <v>#VALUE!</v>
       </c>
       <c r="E15" t="e">
-        <f t="shared" si="9"/>
+        <f>E$13</f>
         <v>#VALUE!</v>
       </c>
       <c r="F15" t="e">
@@ -1285,43 +1285,43 @@
         <f t="shared" si="7"/>
         <v>NA</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="str">
         <f t="shared" si="9"/>
         <v>initial conc (uM)</v>
       </c>
-      <c r="D16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K16" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L16">
+      <c r="D16" s="2" t="e">
+        <f>C16/3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E16" s="2" t="e">
+        <f t="shared" ref="E16:K16" si="10">D16/3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" s="2" t="e">
+        <f>J16/3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L16" s="2">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -1340,39 +1340,39 @@
         <v>NA</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="9"/>
+        <f>C$16</f>
         <v>initial conc (uM)</v>
       </c>
       <c r="D17" t="e">
-        <f t="shared" si="9"/>
+        <f>D$16</f>
         <v>#VALUE!</v>
       </c>
       <c r="E17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="E17:K18" si="11">E$16</f>
         <v>#VALUE!</v>
       </c>
       <c r="F17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="G17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="H17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="I17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="J17" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="K17" t="e">
-        <f t="shared" si="9"/>
+        <f>K$16</f>
         <v>#VALUE!</v>
       </c>
       <c r="L17">
@@ -1394,39 +1394,39 @@
         <v>NA</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="9"/>
+        <f>C$16</f>
         <v>initial conc (uM)</v>
       </c>
       <c r="D18" t="e">
-        <f t="shared" si="9"/>
+        <f>D$16</f>
         <v>#VALUE!</v>
       </c>
       <c r="E18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="F18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="G18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="H18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="I18" t="e">
-        <f t="shared" si="9"/>
+        <f>I$16</f>
         <v>#VALUE!</v>
       </c>
       <c r="J18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="K18" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="L18">
@@ -1501,43 +1501,43 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:L21" si="10">C$1</f>
+        <f t="shared" ref="C21:L21" si="12">C$1</f>
         <v>2</v>
       </c>
       <c r="D21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="E21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="G21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="I21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="J21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="K21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="L21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="M21">
@@ -1555,110 +1555,110 @@
         <v>NA</v>
       </c>
       <c r="C22" s="3" t="str">
-        <f t="shared" ref="B22:M29" si="11">$B$2</f>
+        <f t="shared" ref="B22:M29" si="13">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="E22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="F22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="K22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="L22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="M22" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f t="shared" ref="A23:A29" si="12">A13</f>
+        <f t="shared" ref="A23:A29" si="14">A13</f>
         <v>B</v>
       </c>
       <c r="B23" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" ref="D23:L25" si="13">$C$23</f>
+        <f t="shared" ref="D23:L25" si="15">$C$23</f>
         <v>cell type 1</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="M23" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>C</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C24" t="str">
@@ -1666,53 +1666,53 @@
         <v>cell type 1</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="M24" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>D</v>
       </c>
       <c r="B25" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C25" t="str">
@@ -1720,106 +1720,106 @@
         <v>cell type 1</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>cell type 1</v>
       </c>
       <c r="M25" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>E</v>
       </c>
       <c r="B26" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" ref="D26:L28" si="14">$C$26</f>
+        <f t="shared" ref="D26:L28" si="16">$C$26</f>
         <v>cell type 2</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="M26" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="B27" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C27" t="str">
@@ -1827,53 +1827,53 @@
         <v>cell type 2</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="M27" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>G</v>
       </c>
       <c r="B28" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C28" t="str">
@@ -1881,97 +1881,97 @@
         <v>cell type 2</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>cell type 2</v>
       </c>
       <c r="M28" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>H</v>
       </c>
       <c r="B29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="C29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="H29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="K29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="L29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
       <c r="M29" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -1984,43 +1984,43 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:L41" si="15">C$1</f>
+        <f t="shared" ref="C31:L41" si="17">C$1</f>
         <v>2</v>
       </c>
       <c r="D31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="E31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="F31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="G31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="H31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="I31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="J31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="K31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="L31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
       <c r="M31">
@@ -2030,7 +2030,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f t="shared" ref="A32:A39" si="16">A12</f>
+        <f t="shared" ref="A32:A39" si="18">A12</f>
         <v>A</v>
       </c>
       <c r="B32" s="3" t="str">
@@ -2038,57 +2038,57 @@
         <v>NA</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f t="shared" ref="B32:M39" si="17">$B$2</f>
+        <f t="shared" ref="B32:M39" si="19">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>B</v>
       </c>
       <c r="B33" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C33" s="1"/>
@@ -2102,17 +2102,17 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C</v>
       </c>
       <c r="B34" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C34" s="1"/>
@@ -2126,17 +2126,17 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>D</v>
       </c>
       <c r="B35" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C35" s="1"/>
@@ -2150,17 +2150,17 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>E</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C36" s="1"/>
@@ -2174,17 +2174,17 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>F</v>
       </c>
       <c r="B37" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C37" s="1"/>
@@ -2198,17 +2198,17 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>G</v>
       </c>
       <c r="B38" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C38" s="1"/>
@@ -2222,61 +2222,61 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>H</v>
       </c>
       <c r="B39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
@@ -2289,43 +2289,43 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="D41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="E41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="F41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="G41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="H41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="I41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="J41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="K41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="L41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
       <c r="M41">
@@ -2335,7 +2335,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f t="shared" ref="A42:A49" si="18">A22</f>
+        <f t="shared" ref="A42:A49" si="20">A22</f>
         <v>A</v>
       </c>
       <c r="B42" s="3" t="str">
@@ -2343,425 +2343,425 @@
         <v>NA</v>
       </c>
       <c r="C42" s="3" t="str">
-        <f t="shared" ref="B42:M49" si="19">$B$2</f>
+        <f t="shared" ref="B42:M49" si="21">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="H42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="K42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="L42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="M42" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>B</v>
       </c>
       <c r="B43" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C43" s="2" t="e">
-        <f t="shared" ref="C43:L43" si="20">C33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C43:L43" si="22">C33/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L43" s="2" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C</v>
       </c>
       <c r="B44" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C44" s="2" t="e">
-        <f t="shared" ref="C44:L44" si="21">C34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C44:L44" si="23">C34/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L44" s="2" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M44" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>D</v>
       </c>
       <c r="B45" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C45" s="2" t="e">
-        <f t="shared" ref="C45:L45" si="22">C35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C45:L45" si="24">C35/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L45" s="2" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M45" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>E</v>
       </c>
       <c r="B46" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C46" s="2" t="e">
-        <f t="shared" ref="C46:L46" si="23">C36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C46:L46" si="25">C36/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="2" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>F</v>
       </c>
       <c r="B47" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C47" s="2" t="e">
-        <f t="shared" ref="C47:L47" si="24">C37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C47:L47" si="26">C37/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L47" s="2" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M47" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>G</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C48" s="2" t="e">
-        <f t="shared" ref="C48:L48" si="25">C38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C48:L48" si="27">C38/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L48" s="2" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M48" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>H</v>
       </c>
       <c r="B49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="E49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="H49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="J49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="K49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="L49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
       <c r="M49" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>NA</v>
       </c>
     </row>
@@ -2774,43 +2774,43 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:L51" si="26">C$1</f>
+        <f t="shared" ref="C51:L51" si="28">C$1</f>
         <v>2</v>
       </c>
       <c r="D51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="E51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="F51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
       <c r="G51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>6</v>
       </c>
       <c r="H51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>7</v>
       </c>
       <c r="I51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>8</v>
       </c>
       <c r="J51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9</v>
       </c>
       <c r="K51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="L51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>11</v>
       </c>
       <c r="M51">
@@ -2820,7 +2820,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f t="shared" ref="A52:A59" si="27">A42</f>
+        <f t="shared" ref="A52:A59" si="29">A42</f>
         <v>A</v>
       </c>
       <c r="B52" s="3" t="str">
@@ -2828,57 +2828,57 @@
         <v>NA</v>
       </c>
       <c r="C52" s="3" t="str">
-        <f t="shared" ref="B52:M59" si="28">$B$2</f>
+        <f t="shared" ref="B52:M59" si="30">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="E52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="H52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="I52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="J52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="K52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="L52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="M52" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>B</v>
       </c>
       <c r="B53" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C53">
@@ -2912,17 +2912,17 @@
         <v>1</v>
       </c>
       <c r="M53" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>C</v>
       </c>
       <c r="B54" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C54">
@@ -2956,17 +2956,17 @@
         <v>2</v>
       </c>
       <c r="M54" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>D</v>
       </c>
       <c r="B55" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C55">
@@ -3000,17 +3000,17 @@
         <v>3</v>
       </c>
       <c r="M55" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>E</v>
       </c>
       <c r="B56" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C56">
@@ -3044,17 +3044,17 @@
         <v>1</v>
       </c>
       <c r="M56" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>F</v>
       </c>
       <c r="B57" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C57">
@@ -3088,17 +3088,17 @@
         <v>2</v>
       </c>
       <c r="M57" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>G</v>
       </c>
       <c r="B58" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C58">
@@ -3132,65 +3132,101 @@
         <v>3</v>
       </c>
       <c r="M58" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>H</v>
       </c>
       <c r="B59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="C59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="D59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="H59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="I59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="J59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="K59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="L59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
       <c r="M59" s="3" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>NA</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C13:L18">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:L38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:L48">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated import template color formatting
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D87DD0-C847-0B47-952C-D96C5AB2047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E40BC5-C9BB-CD41-94B6-82F03351D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>B</t>
   </si>
@@ -68,12 +68,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>cell type 1</t>
-  </si>
-  <si>
-    <t>cell type 2</t>
-  </si>
-  <si>
     <t>initial conc (uM)</t>
   </si>
   <si>
@@ -93,6 +87,12 @@
   </si>
   <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>target 1</t>
+  </si>
+  <si>
+    <t>target 2</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4096A825-2A06-5E4B-BFDF-9409981589B8}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -648,7 +648,7 @@
         <v>NA</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:L8" si="2">$C$3</f>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <f>B$1</f>
@@ -1126,7 +1126,7 @@
         <v>NA</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="e">
         <f>C13/3</f>
@@ -1285,16 +1285,15 @@
         <f t="shared" si="7"/>
         <v>NA</v>
       </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>initial conc (uM)</v>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="e">
         <f>C16/3</f>
         <v>#VALUE!</v>
       </c>
       <c r="E16" s="2" t="e">
-        <f t="shared" ref="E16:K16" si="10">D16/3</f>
+        <f t="shared" ref="E16:J16" si="10">D16/3</f>
         <v>#VALUE!</v>
       </c>
       <c r="F16" s="2" t="e">
@@ -1494,7 +1493,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <f>B$1</f>
@@ -1609,43 +1608,43 @@
         <v>NA</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ref="D23:L25" si="15">$C$23</f>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="M23" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1663,43 +1662,43 @@
       </c>
       <c r="C24" t="str">
         <f>$C$23</f>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="M24" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1717,43 +1716,43 @@
       </c>
       <c r="C25" t="str">
         <f>$C$23</f>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="15"/>
-        <v>cell type 1</v>
+        <v>target 1</v>
       </c>
       <c r="M25" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1770,43 +1769,43 @@
         <v>NA</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" ref="D26:L28" si="16">$C$26</f>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="M26" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1824,43 +1823,43 @@
       </c>
       <c r="C27" t="str">
         <f>$C$26</f>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="M27" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1878,43 +1877,43 @@
       </c>
       <c r="C28" t="str">
         <f>$C$26</f>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="16"/>
-        <v>cell type 2</v>
+        <v>target 2</v>
       </c>
       <c r="M28" s="3" t="str">
         <f t="shared" si="13"/>
@@ -1977,7 +1976,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <f>B$1</f>
@@ -2282,7 +2281,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41">
         <f>B$1</f>
@@ -3192,7 +3191,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:L18">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3209,9 +3208,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3221,9 +3220,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Renamed "compound" to "treatment" across everything that I can find. Manual tests seem fine
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F753E-17F6-E643-9B20-FF52D9E8D45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C890803-EFD4-964D-9C62-308813E9CB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>compound</t>
-  </si>
-  <si>
     <t>readout</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>initial conc 2 (uM)</t>
+  </si>
+  <si>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4096A825-2A06-5E4B-BFDF-9409981589B8}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
@@ -639,10 +639,10 @@
         <v>NA</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:L8" si="2">$C$3</f>
+        <f t="shared" ref="D3:L5" si="2">$C$3</f>
         <v>treatment 1</v>
       </c>
       <c r="E3" s="3" t="str">
@@ -797,7 +797,7 @@
         <v>NA</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="str">
         <f>$C$6</f>
@@ -853,7 +853,7 @@
         <v>treatment 2</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f t="shared" ref="D7:L8" si="6">$C$6</f>
+        <f t="shared" ref="D7:D8" si="6">$C$6</f>
         <v>treatment 2</v>
       </c>
       <c r="E7" s="3" t="str">
@@ -1001,7 +1001,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <f>B$1</f>
@@ -1116,7 +1116,7 @@
         <v>NA</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="e">
         <f>C13/3</f>
@@ -1168,7 +1168,7 @@
         <v>NA</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" ref="C14:L18" si="12">C$13</f>
+        <f t="shared" ref="C14:K15" si="12">C$13</f>
         <v>initial conc 1 (uM)</v>
       </c>
       <c r="D14" s="3" t="e">
@@ -1274,7 +1274,7 @@
         <v>NA</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="4" t="e">
         <f>C16/3</f>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2">
         <f>B$1</f>
@@ -1593,7 +1593,7 @@
         <v>NA</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" ref="D23:L25" si="18">$C$23</f>
@@ -1754,7 +1754,7 @@
         <v>NA</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" ref="D26:L28" si="19">$C$26</f>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="2">
         <f>B$1</f>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="2">
         <f>B$1</f>

</xml_diff>

<commit_message>
updated style slightly for reaadable dilutions
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C890803-EFD4-964D-9C62-308813E9CB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4428562-4456-6044-AB15-20EF127D2484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +143,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -162,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -194,27 +202,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Linked Cell" xfId="3" builtinId="24"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,7 +555,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1118,35 +1144,35 @@
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4" t="e">
+      <c r="D13" s="5" t="e">
         <f>C13/3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E13" s="4" t="e">
+      <c r="E13" s="5" t="e">
         <f t="shared" ref="E13:K13" si="11">D13/3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F13" s="4" t="e">
+      <c r="F13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13" s="4" t="e">
+      <c r="G13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H13" s="4" t="e">
+      <c r="H13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I13" s="4" t="e">
+      <c r="I13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J13" s="4" t="e">
+      <c r="J13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K13" s="4" t="e">
+      <c r="K13" s="5" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
@@ -1276,35 +1302,35 @@
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4" t="e">
+      <c r="D16" s="5" t="e">
         <f>C16/3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E16" s="4" t="e">
+      <c r="E16" s="5" t="e">
         <f t="shared" ref="E16:J16" si="13">D16/3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F16" s="4" t="e">
+      <c r="F16" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G16" s="4" t="e">
+      <c r="G16" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H16" s="4" t="e">
+      <c r="H16" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I16" s="4" t="e">
+      <c r="I16" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J16" s="4" t="e">
+      <c r="J16" s="5" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K16" s="4" t="e">
+      <c r="K16" s="5" t="e">
         <f>J16/3</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>